<commit_message>
Gerber parser have been creating
</commit_message>
<xml_diff>
--- a/gerber.xlsx
+++ b/gerber.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>code</t>
   </si>
@@ -128,9 +128,6 @@
     <t>G71</t>
   </si>
   <si>
-    <t>It's default unit</t>
-  </si>
-  <si>
     <t>LP</t>
   </si>
   <si>
@@ -144,6 +141,108 @@
   </si>
   <si>
     <t>Clear o Dark color</t>
+  </si>
+  <si>
+    <t>M02</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>L or T, A or I</t>
+  </si>
+  <si>
+    <t>%FSLAX25Y25*%</t>
+  </si>
+  <si>
+    <t>L or T zeros omitted, A or I Absolute or incremental, XY format of input data</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>equals command MOIN. It's default unit</t>
+  </si>
+  <si>
+    <t>%MOIN%</t>
+  </si>
+  <si>
+    <t>IN or MM</t>
+  </si>
+  <si>
+    <t>Inches or millimeters, default is IN</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>Aperture definition</t>
+  </si>
+  <si>
+    <t>%ADD10C,0.02400*%</t>
+  </si>
+  <si>
+    <t>Documentation https://www.ucamco.com/files/downloads/file/81/the_gerber_file_format_specification.pdf</t>
+  </si>
+  <si>
+    <t>More basic in http://www.artwork.com/gerber/274x/rs274x.htm</t>
+  </si>
+  <si>
+    <t>In basic implementation C and R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C R O P </t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>Aperture Macro. It's complex an not very common</t>
+  </si>
+  <si>
+    <t>G04</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>G54</t>
+  </si>
+  <si>
+    <t>Select aperture</t>
+  </si>
+  <si>
+    <t>G54D10</t>
+  </si>
+  <si>
+    <t>Dxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xx is the tool defined with ADD </t>
+  </si>
+  <si>
+    <t>G36</t>
+  </si>
+  <si>
+    <t>G37</t>
+  </si>
+  <si>
+    <t>Start fill poligon</t>
+  </si>
+  <si>
+    <t>Too many command end in G37 command</t>
+  </si>
+  <si>
+    <t>End G36 command</t>
+  </si>
+  <si>
+    <t>Equals command MOMM.</t>
+  </si>
+  <si>
+    <t>Format specification</t>
   </si>
 </sst>
 </file>
@@ -173,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +296,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -207,13 +312,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -230,10 +336,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="20% - Énfasis5" xfId="2" builtinId="46"/>
+    <cellStyle name="40% - Énfasis5" xfId="4" builtinId="47"/>
     <cellStyle name="60% - Énfasis5" xfId="3" builtinId="48"/>
     <cellStyle name="Énfasis5" xfId="1" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,169 +625,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K11"/>
+  <dimension ref="B1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="D5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="I5" t="s">
+      <c r="D6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="I6" t="s">
         <v>25</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="I6" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="I7" t="s">
         <v>26</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="3" t="s">
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>